<commit_message>
switch Rock Creek-Buck Creek Huc10 to silver lake watershed
</commit_message>
<xml_diff>
--- a/1_fetch/in/lake_huc6_huc8_huc10_structure_table.xlsx
+++ b/1_fetch/in/lake_huc6_huc8_huc10_structure_table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/msleckman/USGS/Vizlab/saline-lakes/1_fetch/in/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{786DA642-8E6B-AC41-9298-BD329F5917A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20EECE6C-27AD-8240-9973-A0BC586F9558}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="43280" yWindow="-6200" windowWidth="35840" windowHeight="19980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10655" uniqueCount="1659">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10575" uniqueCount="1659">
   <si>
     <t>lake_w_state</t>
   </si>
@@ -5078,14 +5078,9 @@
   <autoFilter ref="A1:H1464" xr:uid="{00000000-0009-0000-0100-000003000000}">
     <filterColumn colId="0">
       <filters>
-        <filter val="Harney Lake,OR"/>
-        <filter val="Malheur Lake,OR"/>
+        <filter val="Carson Lake,NV"/>
+        <filter val="Carson Sink,NV"/>
       </filters>
-    </filterColumn>
-    <filterColumn colId="7">
-      <customFilters>
-        <customFilter operator="notEqual" val=" "/>
-      </customFilters>
     </filterColumn>
   </autoFilter>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A835:H1317">
@@ -5386,8 +5381,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H1464"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H1117" sqref="H1117"/>
+    <sheetView tabSelected="1" topLeftCell="A250" workbookViewId="0">
+      <selection activeCell="G301" sqref="G301"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -10455,7 +10450,7 @@
         <v>1639</v>
       </c>
     </row>
-    <row r="201" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
         <v>459</v>
       </c>
@@ -10477,11 +10472,9 @@
       <c r="G201" t="s">
         <v>465</v>
       </c>
-      <c r="H201" s="1" t="s">
-        <v>1639</v>
-      </c>
-    </row>
-    <row r="202" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H201" s="1"/>
+    </row>
+    <row r="202" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
         <v>459</v>
       </c>
@@ -10503,11 +10496,9 @@
       <c r="G202" t="s">
         <v>467</v>
       </c>
-      <c r="H202" s="1" t="s">
-        <v>1639</v>
-      </c>
-    </row>
-    <row r="203" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H202" s="1"/>
+    </row>
+    <row r="203" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
         <v>459</v>
       </c>
@@ -10529,11 +10520,9 @@
       <c r="G203" t="s">
         <v>469</v>
       </c>
-      <c r="H203" s="1" t="s">
-        <v>1639</v>
-      </c>
-    </row>
-    <row r="204" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H203" s="1"/>
+    </row>
+    <row r="204" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A204" t="s">
         <v>459</v>
       </c>
@@ -10555,11 +10544,9 @@
       <c r="G204" t="s">
         <v>473</v>
       </c>
-      <c r="H204" s="1" t="s">
-        <v>1639</v>
-      </c>
-    </row>
-    <row r="205" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H204" s="1"/>
+    </row>
+    <row r="205" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A205" t="s">
         <v>459</v>
       </c>
@@ -10581,11 +10568,9 @@
       <c r="G205" t="s">
         <v>475</v>
       </c>
-      <c r="H205" s="1" t="s">
-        <v>1639</v>
-      </c>
-    </row>
-    <row r="206" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H205" s="1"/>
+    </row>
+    <row r="206" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A206" t="s">
         <v>459</v>
       </c>
@@ -10607,11 +10592,9 @@
       <c r="G206" t="s">
         <v>473</v>
       </c>
-      <c r="H206" s="1" t="s">
-        <v>1639</v>
-      </c>
-    </row>
-    <row r="207" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H206" s="1"/>
+    </row>
+    <row r="207" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A207" t="s">
         <v>459</v>
       </c>
@@ -10633,11 +10616,9 @@
       <c r="G207" t="s">
         <v>482</v>
       </c>
-      <c r="H207" s="1" t="s">
-        <v>1639</v>
-      </c>
-    </row>
-    <row r="208" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H207" s="1"/>
+    </row>
+    <row r="208" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A208" t="s">
         <v>459</v>
       </c>
@@ -10659,11 +10640,9 @@
       <c r="G208" t="s">
         <v>486</v>
       </c>
-      <c r="H208" s="1" t="s">
-        <v>1639</v>
-      </c>
-    </row>
-    <row r="209" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H208" s="1"/>
+    </row>
+    <row r="209" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A209" t="s">
         <v>459</v>
       </c>
@@ -10685,11 +10664,9 @@
       <c r="G209" t="s">
         <v>490</v>
       </c>
-      <c r="H209" s="1" t="s">
-        <v>1639</v>
-      </c>
-    </row>
-    <row r="210" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H209" s="1"/>
+    </row>
+    <row r="210" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A210" t="s">
         <v>459</v>
       </c>
@@ -10711,11 +10688,9 @@
       <c r="G210" t="s">
         <v>492</v>
       </c>
-      <c r="H210" s="1" t="s">
-        <v>1639</v>
-      </c>
-    </row>
-    <row r="211" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H210" s="1"/>
+    </row>
+    <row r="211" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A211" t="s">
         <v>459</v>
       </c>
@@ -10737,11 +10712,9 @@
       <c r="G211" t="s">
         <v>494</v>
       </c>
-      <c r="H211" s="1" t="s">
-        <v>1639</v>
-      </c>
-    </row>
-    <row r="212" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H211" s="1"/>
+    </row>
+    <row r="212" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A212" t="s">
         <v>459</v>
       </c>
@@ -10763,11 +10736,9 @@
       <c r="G212" t="s">
         <v>496</v>
       </c>
-      <c r="H212" s="1" t="s">
-        <v>1639</v>
-      </c>
-    </row>
-    <row r="213" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H212" s="1"/>
+    </row>
+    <row r="213" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A213" t="s">
         <v>459</v>
       </c>
@@ -10789,11 +10760,9 @@
       <c r="G213" t="s">
         <v>498</v>
       </c>
-      <c r="H213" s="1" t="s">
-        <v>1639</v>
-      </c>
-    </row>
-    <row r="214" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H213" s="1"/>
+    </row>
+    <row r="214" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A214" t="s">
         <v>459</v>
       </c>
@@ -10815,11 +10784,9 @@
       <c r="G214" t="s">
         <v>502</v>
       </c>
-      <c r="H214" s="1" t="s">
-        <v>1639</v>
-      </c>
-    </row>
-    <row r="215" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H214" s="1"/>
+    </row>
+    <row r="215" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A215" t="s">
         <v>459</v>
       </c>
@@ -10841,11 +10808,9 @@
       <c r="G215" t="s">
         <v>504</v>
       </c>
-      <c r="H215" s="1" t="s">
-        <v>1639</v>
-      </c>
-    </row>
-    <row r="216" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H215" s="1"/>
+    </row>
+    <row r="216" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A216" t="s">
         <v>459</v>
       </c>
@@ -10867,11 +10832,9 @@
       <c r="G216" t="s">
         <v>506</v>
       </c>
-      <c r="H216" s="1" t="s">
-        <v>1639</v>
-      </c>
-    </row>
-    <row r="217" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H216" s="1"/>
+    </row>
+    <row r="217" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A217" t="s">
         <v>459</v>
       </c>
@@ -10893,11 +10856,9 @@
       <c r="G217" t="s">
         <v>508</v>
       </c>
-      <c r="H217" s="1" t="s">
-        <v>1639</v>
-      </c>
-    </row>
-    <row r="218" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H217" s="1"/>
+    </row>
+    <row r="218" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A218" t="s">
         <v>459</v>
       </c>
@@ -10919,11 +10880,9 @@
       <c r="G218" t="s">
         <v>510</v>
       </c>
-      <c r="H218" s="1" t="s">
-        <v>1639</v>
-      </c>
-    </row>
-    <row r="219" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H218" s="1"/>
+    </row>
+    <row r="219" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A219" t="s">
         <v>459</v>
       </c>
@@ -10945,11 +10904,9 @@
       <c r="G219" t="s">
         <v>512</v>
       </c>
-      <c r="H219" s="1" t="s">
-        <v>1639</v>
-      </c>
-    </row>
-    <row r="220" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H219" s="1"/>
+    </row>
+    <row r="220" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A220" t="s">
         <v>459</v>
       </c>
@@ -10971,11 +10928,9 @@
       <c r="G220" t="s">
         <v>514</v>
       </c>
-      <c r="H220" s="1" t="s">
-        <v>1639</v>
-      </c>
-    </row>
-    <row r="221" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H220" s="1"/>
+    </row>
+    <row r="221" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A221" t="s">
         <v>459</v>
       </c>
@@ -10997,11 +10952,9 @@
       <c r="G221" t="s">
         <v>516</v>
       </c>
-      <c r="H221" s="1" t="s">
-        <v>1639</v>
-      </c>
-    </row>
-    <row r="222" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H221" s="1"/>
+    </row>
+    <row r="222" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A222" t="s">
         <v>459</v>
       </c>
@@ -11023,11 +10976,9 @@
       <c r="G222" t="s">
         <v>518</v>
       </c>
-      <c r="H222" s="1" t="s">
-        <v>1639</v>
-      </c>
-    </row>
-    <row r="223" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H222" s="1"/>
+    </row>
+    <row r="223" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A223" t="s">
         <v>459</v>
       </c>
@@ -11049,11 +11000,9 @@
       <c r="G223" t="s">
         <v>520</v>
       </c>
-      <c r="H223" s="1" t="s">
-        <v>1639</v>
-      </c>
-    </row>
-    <row r="224" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H223" s="1"/>
+    </row>
+    <row r="224" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A224" t="s">
         <v>459</v>
       </c>
@@ -11075,11 +11024,9 @@
       <c r="G224" t="s">
         <v>522</v>
       </c>
-      <c r="H224" s="1" t="s">
-        <v>1639</v>
-      </c>
-    </row>
-    <row r="225" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H224" s="1"/>
+    </row>
+    <row r="225" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A225" t="s">
         <v>459</v>
       </c>
@@ -11101,11 +11048,9 @@
       <c r="G225" t="s">
         <v>524</v>
       </c>
-      <c r="H225" s="1" t="s">
-        <v>1639</v>
-      </c>
-    </row>
-    <row r="226" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H225" s="1"/>
+    </row>
+    <row r="226" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A226" t="s">
         <v>459</v>
       </c>
@@ -11127,11 +11072,9 @@
       <c r="G226" t="s">
         <v>526</v>
       </c>
-      <c r="H226" s="1" t="s">
-        <v>1639</v>
-      </c>
-    </row>
-    <row r="227" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H226" s="1"/>
+    </row>
+    <row r="227" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A227" t="s">
         <v>459</v>
       </c>
@@ -11153,11 +11096,9 @@
       <c r="G227" t="s">
         <v>528</v>
       </c>
-      <c r="H227" s="1" t="s">
-        <v>1639</v>
-      </c>
-    </row>
-    <row r="228" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H227" s="1"/>
+    </row>
+    <row r="228" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A228" t="s">
         <v>459</v>
       </c>
@@ -11179,11 +11120,9 @@
       <c r="G228" t="s">
         <v>530</v>
       </c>
-      <c r="H228" s="1" t="s">
-        <v>1639</v>
-      </c>
-    </row>
-    <row r="229" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H228" s="1"/>
+    </row>
+    <row r="229" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A229" t="s">
         <v>459</v>
       </c>
@@ -11205,11 +11144,9 @@
       <c r="G229" t="s">
         <v>532</v>
       </c>
-      <c r="H229" s="1" t="s">
-        <v>1639</v>
-      </c>
-    </row>
-    <row r="230" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H229" s="1"/>
+    </row>
+    <row r="230" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A230" t="s">
         <v>459</v>
       </c>
@@ -11231,11 +11168,9 @@
       <c r="G230" t="s">
         <v>534</v>
       </c>
-      <c r="H230" s="1" t="s">
-        <v>1639</v>
-      </c>
-    </row>
-    <row r="231" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H230" s="1"/>
+    </row>
+    <row r="231" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A231" t="s">
         <v>459</v>
       </c>
@@ -11257,11 +11192,9 @@
       <c r="G231" t="s">
         <v>536</v>
       </c>
-      <c r="H231" s="1" t="s">
-        <v>1639</v>
-      </c>
-    </row>
-    <row r="232" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H231" s="1"/>
+    </row>
+    <row r="232" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A232" t="s">
         <v>459</v>
       </c>
@@ -11283,11 +11216,9 @@
       <c r="G232" t="s">
         <v>538</v>
       </c>
-      <c r="H232" s="1" t="s">
-        <v>1639</v>
-      </c>
-    </row>
-    <row r="233" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H232" s="1"/>
+    </row>
+    <row r="233" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A233" t="s">
         <v>459</v>
       </c>
@@ -11309,11 +11240,9 @@
       <c r="G233" t="s">
         <v>542</v>
       </c>
-      <c r="H233" s="1" t="s">
-        <v>1639</v>
-      </c>
-    </row>
-    <row r="234" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H233" s="1"/>
+    </row>
+    <row r="234" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A234" t="s">
         <v>459</v>
       </c>
@@ -11335,11 +11264,9 @@
       <c r="G234" t="s">
         <v>544</v>
       </c>
-      <c r="H234" s="1" t="s">
-        <v>1639</v>
-      </c>
-    </row>
-    <row r="235" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H234" s="1"/>
+    </row>
+    <row r="235" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A235" t="s">
         <v>459</v>
       </c>
@@ -11361,11 +11288,9 @@
       <c r="G235" t="s">
         <v>546</v>
       </c>
-      <c r="H235" s="1" t="s">
-        <v>1639</v>
-      </c>
-    </row>
-    <row r="236" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H235" s="1"/>
+    </row>
+    <row r="236" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A236" t="s">
         <v>459</v>
       </c>
@@ -11387,11 +11312,9 @@
       <c r="G236" t="s">
         <v>550</v>
       </c>
-      <c r="H236" s="1" t="s">
-        <v>1639</v>
-      </c>
-    </row>
-    <row r="237" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H236" s="1"/>
+    </row>
+    <row r="237" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A237" t="s">
         <v>459</v>
       </c>
@@ -11413,11 +11336,9 @@
       <c r="G237" t="s">
         <v>199</v>
       </c>
-      <c r="H237" s="1" t="s">
-        <v>1639</v>
-      </c>
-    </row>
-    <row r="238" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H237" s="1"/>
+    </row>
+    <row r="238" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A238" t="s">
         <v>459</v>
       </c>
@@ -11439,11 +11360,9 @@
       <c r="G238" t="s">
         <v>553</v>
       </c>
-      <c r="H238" s="1" t="s">
-        <v>1639</v>
-      </c>
-    </row>
-    <row r="239" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H238" s="1"/>
+    </row>
+    <row r="239" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A239" t="s">
         <v>459</v>
       </c>
@@ -11465,11 +11384,9 @@
       <c r="G239" t="s">
         <v>555</v>
       </c>
-      <c r="H239" s="1" t="s">
-        <v>1639</v>
-      </c>
-    </row>
-    <row r="240" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H239" s="1"/>
+    </row>
+    <row r="240" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A240" t="s">
         <v>459</v>
       </c>
@@ -11491,11 +11408,9 @@
       <c r="G240" t="s">
         <v>557</v>
       </c>
-      <c r="H240" s="1" t="s">
-        <v>1639</v>
-      </c>
-    </row>
-    <row r="241" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H240" s="1"/>
+    </row>
+    <row r="241" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A241" t="s">
         <v>459</v>
       </c>
@@ -11517,11 +11432,9 @@
       <c r="G241" t="s">
         <v>559</v>
       </c>
-      <c r="H241" s="1" t="s">
-        <v>1639</v>
-      </c>
-    </row>
-    <row r="242" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H241" s="1"/>
+    </row>
+    <row r="242" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A242" t="s">
         <v>459</v>
       </c>
@@ -11543,11 +11456,9 @@
       <c r="G242" t="s">
         <v>561</v>
       </c>
-      <c r="H242" s="1" t="s">
-        <v>1639</v>
-      </c>
-    </row>
-    <row r="243" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H242" s="1"/>
+    </row>
+    <row r="243" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A243" t="s">
         <v>459</v>
       </c>
@@ -11569,11 +11480,9 @@
       <c r="G243" t="s">
         <v>563</v>
       </c>
-      <c r="H243" s="1" t="s">
-        <v>1639</v>
-      </c>
-    </row>
-    <row r="244" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H243" s="1"/>
+    </row>
+    <row r="244" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A244" t="s">
         <v>459</v>
       </c>
@@ -11595,11 +11504,9 @@
       <c r="G244" t="s">
         <v>565</v>
       </c>
-      <c r="H244" s="1" t="s">
-        <v>1639</v>
-      </c>
-    </row>
-    <row r="245" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H244" s="1"/>
+    </row>
+    <row r="245" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A245" t="s">
         <v>459</v>
       </c>
@@ -11621,11 +11528,9 @@
       <c r="G245" t="s">
         <v>567</v>
       </c>
-      <c r="H245" s="1" t="s">
-        <v>1639</v>
-      </c>
-    </row>
-    <row r="246" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H245" s="1"/>
+    </row>
+    <row r="246" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A246" t="s">
         <v>459</v>
       </c>
@@ -11647,11 +11552,9 @@
       <c r="G246" t="s">
         <v>569</v>
       </c>
-      <c r="H246" s="1" t="s">
-        <v>1639</v>
-      </c>
-    </row>
-    <row r="247" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H246" s="1"/>
+    </row>
+    <row r="247" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A247" t="s">
         <v>459</v>
       </c>
@@ -11673,11 +11576,9 @@
       <c r="G247" t="s">
         <v>571</v>
       </c>
-      <c r="H247" s="1" t="s">
-        <v>1639</v>
-      </c>
-    </row>
-    <row r="248" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H247" s="1"/>
+    </row>
+    <row r="248" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A248" t="s">
         <v>459</v>
       </c>
@@ -11699,11 +11600,9 @@
       <c r="G248" t="s">
         <v>573</v>
       </c>
-      <c r="H248" s="1" t="s">
-        <v>1639</v>
-      </c>
-    </row>
-    <row r="249" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H248" s="1"/>
+    </row>
+    <row r="249" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A249" t="s">
         <v>459</v>
       </c>
@@ -11725,11 +11624,9 @@
       <c r="G249" t="s">
         <v>575</v>
       </c>
-      <c r="H249" s="1" t="s">
-        <v>1639</v>
-      </c>
-    </row>
-    <row r="250" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H249" s="1"/>
+    </row>
+    <row r="250" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A250" t="s">
         <v>459</v>
       </c>
@@ -11751,11 +11648,9 @@
       <c r="G250" t="s">
         <v>577</v>
       </c>
-      <c r="H250" s="1" t="s">
-        <v>1639</v>
-      </c>
-    </row>
-    <row r="251" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H250" s="1"/>
+    </row>
+    <row r="251" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A251" t="s">
         <v>459</v>
       </c>
@@ -11777,11 +11672,9 @@
       <c r="G251" t="s">
         <v>391</v>
       </c>
-      <c r="H251" s="1" t="s">
-        <v>1639</v>
-      </c>
-    </row>
-    <row r="252" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H251" s="1"/>
+    </row>
+    <row r="252" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A252" t="s">
         <v>459</v>
       </c>
@@ -11803,11 +11696,9 @@
       <c r="G252" t="s">
         <v>580</v>
       </c>
-      <c r="H252" s="1" t="s">
-        <v>1639</v>
-      </c>
-    </row>
-    <row r="253" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H252" s="1"/>
+    </row>
+    <row r="253" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A253" t="s">
         <v>459</v>
       </c>
@@ -11829,11 +11720,9 @@
       <c r="G253" t="s">
         <v>582</v>
       </c>
-      <c r="H253" s="1" t="s">
-        <v>1639</v>
-      </c>
-    </row>
-    <row r="254" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H253" s="1"/>
+    </row>
+    <row r="254" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A254" t="s">
         <v>459</v>
       </c>
@@ -11855,11 +11744,9 @@
       <c r="G254" t="s">
         <v>467</v>
       </c>
-      <c r="H254" s="1" t="s">
-        <v>1639</v>
-      </c>
-    </row>
-    <row r="255" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H254" s="1"/>
+    </row>
+    <row r="255" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A255" t="s">
         <v>459</v>
       </c>
@@ -11881,11 +11768,9 @@
       <c r="G255" t="s">
         <v>585</v>
       </c>
-      <c r="H255" s="1" t="s">
-        <v>1639</v>
-      </c>
-    </row>
-    <row r="256" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H255" s="1"/>
+    </row>
+    <row r="256" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A256" t="s">
         <v>459</v>
       </c>
@@ -11907,11 +11792,9 @@
       <c r="G256" t="s">
         <v>587</v>
       </c>
-      <c r="H256" s="1" t="s">
-        <v>1639</v>
-      </c>
-    </row>
-    <row r="257" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H256" s="1"/>
+    </row>
+    <row r="257" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A257" t="s">
         <v>459</v>
       </c>
@@ -11933,11 +11816,9 @@
       <c r="G257" t="s">
         <v>589</v>
       </c>
-      <c r="H257" s="1" t="s">
-        <v>1639</v>
-      </c>
-    </row>
-    <row r="258" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H257" s="1"/>
+    </row>
+    <row r="258" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A258" t="s">
         <v>459</v>
       </c>
@@ -11959,11 +11840,9 @@
       <c r="G258" t="s">
         <v>591</v>
       </c>
-      <c r="H258" s="1" t="s">
-        <v>1639</v>
-      </c>
-    </row>
-    <row r="259" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H258" s="1"/>
+    </row>
+    <row r="259" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A259" t="s">
         <v>459</v>
       </c>
@@ -11985,11 +11864,9 @@
       <c r="G259" t="s">
         <v>593</v>
       </c>
-      <c r="H259" s="1" t="s">
-        <v>1639</v>
-      </c>
-    </row>
-    <row r="260" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H259" s="1"/>
+    </row>
+    <row r="260" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A260" t="s">
         <v>459</v>
       </c>
@@ -12011,11 +11888,9 @@
       <c r="G260" t="s">
         <v>595</v>
       </c>
-      <c r="H260" s="1" t="s">
-        <v>1639</v>
-      </c>
-    </row>
-    <row r="261" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H260" s="1"/>
+    </row>
+    <row r="261" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A261" t="s">
         <v>459</v>
       </c>
@@ -12037,11 +11912,9 @@
       <c r="G261" t="s">
         <v>597</v>
       </c>
-      <c r="H261" s="1" t="s">
-        <v>1639</v>
-      </c>
-    </row>
-    <row r="262" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H261" s="1"/>
+    </row>
+    <row r="262" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A262" t="s">
         <v>459</v>
       </c>
@@ -12063,11 +11936,9 @@
       <c r="G262" t="s">
         <v>599</v>
       </c>
-      <c r="H262" s="1" t="s">
-        <v>1639</v>
-      </c>
-    </row>
-    <row r="263" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H262" s="1"/>
+    </row>
+    <row r="263" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A263" t="s">
         <v>459</v>
       </c>
@@ -12089,11 +11960,9 @@
       <c r="G263" t="s">
         <v>601</v>
       </c>
-      <c r="H263" s="1" t="s">
-        <v>1639</v>
-      </c>
-    </row>
-    <row r="264" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H263" s="1"/>
+    </row>
+    <row r="264" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A264" t="s">
         <v>459</v>
       </c>
@@ -12115,11 +11984,9 @@
       <c r="G264" t="s">
         <v>603</v>
       </c>
-      <c r="H264" s="1" t="s">
-        <v>1639</v>
-      </c>
-    </row>
-    <row r="265" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H264" s="1"/>
+    </row>
+    <row r="265" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A265" t="s">
         <v>459</v>
       </c>
@@ -12141,11 +12008,9 @@
       <c r="G265" t="s">
         <v>605</v>
       </c>
-      <c r="H265" s="1" t="s">
-        <v>1639</v>
-      </c>
-    </row>
-    <row r="266" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H265" s="1"/>
+    </row>
+    <row r="266" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A266" t="s">
         <v>459</v>
       </c>
@@ -12167,11 +12032,9 @@
       <c r="G266" t="s">
         <v>607</v>
       </c>
-      <c r="H266" s="1" t="s">
-        <v>1639</v>
-      </c>
-    </row>
-    <row r="267" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H266" s="1"/>
+    </row>
+    <row r="267" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A267" t="s">
         <v>459</v>
       </c>
@@ -12193,11 +12056,9 @@
       <c r="G267" t="s">
         <v>609</v>
       </c>
-      <c r="H267" s="1" t="s">
-        <v>1639</v>
-      </c>
-    </row>
-    <row r="268" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H267" s="1"/>
+    </row>
+    <row r="268" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A268" t="s">
         <v>459</v>
       </c>
@@ -12219,11 +12080,9 @@
       <c r="G268" t="s">
         <v>611</v>
       </c>
-      <c r="H268" s="1" t="s">
-        <v>1639</v>
-      </c>
-    </row>
-    <row r="269" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H268" s="1"/>
+    </row>
+    <row r="269" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A269" t="s">
         <v>459</v>
       </c>
@@ -12245,11 +12104,9 @@
       <c r="G269" t="s">
         <v>613</v>
       </c>
-      <c r="H269" s="1" t="s">
-        <v>1639</v>
-      </c>
-    </row>
-    <row r="270" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H269" s="1"/>
+    </row>
+    <row r="270" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A270" t="s">
         <v>459</v>
       </c>
@@ -12271,11 +12128,9 @@
       <c r="G270" t="s">
         <v>615</v>
       </c>
-      <c r="H270" s="1" t="s">
-        <v>1639</v>
-      </c>
-    </row>
-    <row r="271" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H270" s="1"/>
+    </row>
+    <row r="271" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A271" t="s">
         <v>459</v>
       </c>
@@ -12297,11 +12152,9 @@
       <c r="G271" t="s">
         <v>617</v>
       </c>
-      <c r="H271" s="1" t="s">
-        <v>1639</v>
-      </c>
-    </row>
-    <row r="272" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H271" s="1"/>
+    </row>
+    <row r="272" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A272" t="s">
         <v>459</v>
       </c>
@@ -12323,11 +12176,9 @@
       <c r="G272" t="s">
         <v>619</v>
       </c>
-      <c r="H272" s="1" t="s">
-        <v>1639</v>
-      </c>
-    </row>
-    <row r="273" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H272" s="1"/>
+    </row>
+    <row r="273" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A273" t="s">
         <v>459</v>
       </c>
@@ -12349,11 +12200,9 @@
       <c r="G273" t="s">
         <v>621</v>
       </c>
-      <c r="H273" s="1" t="s">
-        <v>1639</v>
-      </c>
-    </row>
-    <row r="274" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H273" s="1"/>
+    </row>
+    <row r="274" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A274" t="s">
         <v>459</v>
       </c>
@@ -12375,11 +12224,9 @@
       <c r="G274" t="s">
         <v>623</v>
       </c>
-      <c r="H274" s="1" t="s">
-        <v>1639</v>
-      </c>
-    </row>
-    <row r="275" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H274" s="1"/>
+    </row>
+    <row r="275" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A275" t="s">
         <v>459</v>
       </c>
@@ -12401,11 +12248,9 @@
       <c r="G275" t="s">
         <v>625</v>
       </c>
-      <c r="H275" s="1" t="s">
-        <v>1639</v>
-      </c>
-    </row>
-    <row r="276" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H275" s="1"/>
+    </row>
+    <row r="276" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A276" t="s">
         <v>459</v>
       </c>
@@ -12427,11 +12272,9 @@
       <c r="G276" t="s">
         <v>627</v>
       </c>
-      <c r="H276" s="1" t="s">
-        <v>1639</v>
-      </c>
-    </row>
-    <row r="277" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H276" s="1"/>
+    </row>
+    <row r="277" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A277" t="s">
         <v>459</v>
       </c>
@@ -12453,11 +12296,9 @@
       <c r="G277" t="s">
         <v>629</v>
       </c>
-      <c r="H277" s="1" t="s">
-        <v>1639</v>
-      </c>
-    </row>
-    <row r="278" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H277" s="1"/>
+    </row>
+    <row r="278" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A278" t="s">
         <v>459</v>
       </c>
@@ -12479,11 +12320,9 @@
       <c r="G278" t="s">
         <v>631</v>
       </c>
-      <c r="H278" s="1" t="s">
-        <v>1639</v>
-      </c>
-    </row>
-    <row r="279" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H278" s="1"/>
+    </row>
+    <row r="279" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A279" t="s">
         <v>459</v>
       </c>
@@ -12505,9 +12344,7 @@
       <c r="G279" t="s">
         <v>633</v>
       </c>
-      <c r="H279" s="1" t="s">
-        <v>1639</v>
-      </c>
+      <c r="H279" s="1"/>
     </row>
     <row r="280" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A280" t="s">
@@ -12558,7 +12395,7 @@
         <v>638</v>
       </c>
     </row>
-    <row r="282" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="282" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A282" t="s">
         <v>641</v>
       </c>
@@ -12584,7 +12421,7 @@
         <v>1639</v>
       </c>
     </row>
-    <row r="283" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="283" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A283" t="s">
         <v>459</v>
       </c>
@@ -13034,7 +12871,7 @@
         <v>1639</v>
       </c>
     </row>
-    <row r="301" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="301" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A301" t="s">
         <v>641</v>
       </c>
@@ -13060,7 +12897,7 @@
         <v>1639</v>
       </c>
     </row>
-    <row r="302" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="302" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A302" t="s">
         <v>459</v>
       </c>
@@ -13135,7 +12972,7 @@
         <v>688</v>
       </c>
     </row>
-    <row r="305" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="305" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A305" t="s">
         <v>641</v>
       </c>
@@ -13161,7 +12998,7 @@
         <v>1639</v>
       </c>
     </row>
-    <row r="306" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="306" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A306" t="s">
         <v>459</v>
       </c>
@@ -13187,7 +13024,7 @@
         <v>1639</v>
       </c>
     </row>
-    <row r="307" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="307" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A307" t="s">
         <v>641</v>
       </c>
@@ -13213,7 +13050,7 @@
         <v>1639</v>
       </c>
     </row>
-    <row r="308" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="308" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A308" t="s">
         <v>459</v>
       </c>
@@ -13363,7 +13200,7 @@
         <v>1639</v>
       </c>
     </row>
-    <row r="314" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="314" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A314" t="s">
         <v>641</v>
       </c>
@@ -13389,7 +13226,7 @@
         <v>1639</v>
       </c>
     </row>
-    <row r="315" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="315" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A315" t="s">
         <v>459</v>
       </c>
@@ -13415,7 +13252,7 @@
         <v>1639</v>
       </c>
     </row>
-    <row r="316" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="316" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A316" t="s">
         <v>641</v>
       </c>
@@ -13441,7 +13278,7 @@
         <v>1639</v>
       </c>
     </row>
-    <row r="317" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="317" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A317" t="s">
         <v>459</v>
       </c>
@@ -13565,7 +13402,7 @@
         <v>708</v>
       </c>
     </row>
-    <row r="322" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="322" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A322" t="s">
         <v>641</v>
       </c>
@@ -13591,7 +13428,7 @@
         <v>1639</v>
       </c>
     </row>
-    <row r="323" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="323" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A323" t="s">
         <v>459</v>
       </c>
@@ -13617,7 +13454,7 @@
         <v>1639</v>
       </c>
     </row>
-    <row r="324" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="324" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A324" t="s">
         <v>641</v>
       </c>
@@ -13643,7 +13480,7 @@
         <v>1639</v>
       </c>
     </row>
-    <row r="325" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="325" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A325" t="s">
         <v>459</v>
       </c>
@@ -13669,7 +13506,7 @@
         <v>1639</v>
       </c>
     </row>
-    <row r="326" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="326" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A326" t="s">
         <v>641</v>
       </c>
@@ -13695,7 +13532,7 @@
         <v>1639</v>
       </c>
     </row>
-    <row r="327" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="327" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A327" t="s">
         <v>459</v>
       </c>
@@ -13721,7 +13558,7 @@
         <v>1639</v>
       </c>
     </row>
-    <row r="328" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="328" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A328" t="s">
         <v>641</v>
       </c>
@@ -13747,7 +13584,7 @@
         <v>1639</v>
       </c>
     </row>
-    <row r="329" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="329" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A329" t="s">
         <v>459</v>
       </c>
@@ -13822,7 +13659,7 @@
         <v>718</v>
       </c>
     </row>
-    <row r="332" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="332" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A332" t="s">
         <v>641</v>
       </c>
@@ -13848,7 +13685,7 @@
         <v>1639</v>
       </c>
     </row>
-    <row r="333" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="333" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A333" t="s">
         <v>459</v>
       </c>
@@ -13874,7 +13711,7 @@
         <v>1639</v>
       </c>
     </row>
-    <row r="334" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="334" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A334" t="s">
         <v>641</v>
       </c>
@@ -13900,7 +13737,7 @@
         <v>1639</v>
       </c>
     </row>
-    <row r="335" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="335" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A335" t="s">
         <v>459</v>
       </c>
@@ -14102,7 +13939,7 @@
         <v>733</v>
       </c>
     </row>
-    <row r="343" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="343" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A343" t="s">
         <v>641</v>
       </c>
@@ -14128,7 +13965,7 @@
         <v>1639</v>
       </c>
     </row>
-    <row r="344" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="344" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A344" t="s">
         <v>459</v>
       </c>
@@ -14255,7 +14092,7 @@
         <v>1639</v>
       </c>
     </row>
-    <row r="349" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="349" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A349" t="s">
         <v>641</v>
       </c>
@@ -14281,7 +14118,7 @@
         <v>1639</v>
       </c>
     </row>
-    <row r="350" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="350" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A350" t="s">
         <v>459</v>
       </c>
@@ -14307,7 +14144,7 @@
         <v>1639</v>
       </c>
     </row>
-    <row r="351" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="351" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A351" t="s">
         <v>641</v>
       </c>
@@ -14333,7 +14170,7 @@
         <v>1639</v>
       </c>
     </row>
-    <row r="352" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="352" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A352" t="s">
         <v>459</v>
       </c>
@@ -14483,7 +14320,7 @@
         <v>1639</v>
       </c>
     </row>
-    <row r="358" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="358" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A358" t="s">
         <v>641</v>
       </c>
@@ -14509,7 +14346,7 @@
         <v>1639</v>
       </c>
     </row>
-    <row r="359" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="359" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A359" t="s">
         <v>459</v>
       </c>
@@ -14711,7 +14548,7 @@
         <v>1639</v>
       </c>
     </row>
-    <row r="367" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="367" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A367" t="s">
         <v>641</v>
       </c>
@@ -14737,7 +14574,7 @@
         <v>1639</v>
       </c>
     </row>
-    <row r="368" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="368" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A368" t="s">
         <v>459</v>
       </c>
@@ -14916,7 +14753,7 @@
         <v>1639</v>
       </c>
     </row>
-    <row r="375" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="375" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A375" t="s">
         <v>641</v>
       </c>
@@ -14942,7 +14779,7 @@
         <v>1639</v>
       </c>
     </row>
-    <row r="376" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="376" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A376" t="s">
         <v>459</v>
       </c>
@@ -14968,7 +14805,7 @@
         <v>1639</v>
       </c>
     </row>
-    <row r="377" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="377" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A377" t="s">
         <v>641</v>
       </c>
@@ -14994,7 +14831,7 @@
         <v>1639</v>
       </c>
     </row>
-    <row r="378" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="378" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A378" t="s">
         <v>459</v>
       </c>
@@ -25541,7 +25378,7 @@
         <v>1261</v>
       </c>
     </row>
-    <row r="835" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="835" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A835" t="s">
         <v>1270</v>
       </c>
@@ -25593,7 +25430,7 @@
         <v>1639</v>
       </c>
     </row>
-    <row r="837" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="837" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A837" t="s">
         <v>1270</v>
       </c>
@@ -25688,7 +25525,7 @@
         <v>1268</v>
       </c>
     </row>
-    <row r="841" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="841" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A841" t="s">
         <v>1270</v>
       </c>
@@ -25737,7 +25574,7 @@
         <v>1277</v>
       </c>
     </row>
-    <row r="843" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="843" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A843" t="s">
         <v>1270</v>
       </c>
@@ -25832,7 +25669,7 @@
         <v>1277</v>
       </c>
     </row>
-    <row r="847" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="847" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A847" t="s">
         <v>1270</v>
       </c>
@@ -25881,7 +25718,7 @@
         <v>1281</v>
       </c>
     </row>
-    <row r="849" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="849" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A849" t="s">
         <v>1270</v>
       </c>
@@ -25979,7 +25816,7 @@
         <v>1281</v>
       </c>
     </row>
-    <row r="853" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="853" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A853" t="s">
         <v>1270</v>
       </c>
@@ -26028,7 +25865,7 @@
         <v>1283</v>
       </c>
     </row>
-    <row r="855" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="855" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A855" t="s">
         <v>1270</v>
       </c>
@@ -26126,7 +25963,7 @@
         <v>1283</v>
       </c>
     </row>
-    <row r="859" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="859" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A859" t="s">
         <v>1270</v>
       </c>
@@ -26178,7 +26015,7 @@
         <v>1639</v>
       </c>
     </row>
-    <row r="861" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="861" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A861" t="s">
         <v>1270</v>
       </c>
@@ -26273,7 +26110,7 @@
         <v>1285</v>
       </c>
     </row>
-    <row r="865" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="865" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A865" t="s">
         <v>1270</v>
       </c>
@@ -26322,7 +26159,7 @@
         <v>1289</v>
       </c>
     </row>
-    <row r="867" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="867" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A867" t="s">
         <v>1270</v>
       </c>
@@ -26420,7 +26257,7 @@
         <v>1639</v>
       </c>
     </row>
-    <row r="871" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="871" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A871" t="s">
         <v>1270</v>
       </c>
@@ -26469,7 +26306,7 @@
         <v>1291</v>
       </c>
     </row>
-    <row r="873" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="873" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A873" t="s">
         <v>1270</v>
       </c>
@@ -26567,7 +26404,7 @@
         <v>1291</v>
       </c>
     </row>
-    <row r="877" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="877" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A877" t="s">
         <v>1270</v>
       </c>
@@ -26616,7 +26453,7 @@
         <v>1295</v>
       </c>
     </row>
-    <row r="879" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="879" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A879" t="s">
         <v>1270</v>
       </c>
@@ -26711,7 +26548,7 @@
         <v>1295</v>
       </c>
     </row>
-    <row r="883" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="883" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A883" t="s">
         <v>1270</v>
       </c>
@@ -26760,7 +26597,7 @@
         <v>1121</v>
       </c>
     </row>
-    <row r="885" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="885" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A885" t="s">
         <v>1270</v>
       </c>
@@ -27324,7 +27161,7 @@
         <v>1639</v>
       </c>
     </row>
-    <row r="909" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="909" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A909" t="s">
         <v>1270</v>
       </c>
@@ -27601,7 +27438,7 @@
         <v>1310</v>
       </c>
     </row>
-    <row r="921" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="921" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A921" t="s">
         <v>1270</v>
       </c>
@@ -27740,7 +27577,7 @@
         <v>1312</v>
       </c>
     </row>
-    <row r="927" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="927" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A927" t="s">
         <v>1270</v>
       </c>
@@ -27879,7 +27716,7 @@
         <v>1314</v>
       </c>
     </row>
-    <row r="933" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="933" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A933" t="s">
         <v>1270</v>
       </c>
@@ -28156,7 +27993,7 @@
         <v>1318</v>
       </c>
     </row>
-    <row r="945" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="945" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A945" t="s">
         <v>1270</v>
       </c>
@@ -29361,7 +29198,7 @@
         <v>1337</v>
       </c>
     </row>
-    <row r="997" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="997" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A997" t="s">
         <v>1270</v>
       </c>
@@ -29924,7 +29761,7 @@
         <v>1639</v>
       </c>
     </row>
-    <row r="1021" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1021" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1021" t="s">
         <v>1270</v>
       </c>
@@ -30207,7 +30044,7 @@
         <v>1351</v>
       </c>
     </row>
-    <row r="1033" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1033" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1033" t="s">
         <v>1270</v>
       </c>
@@ -30672,7 +30509,7 @@
         <v>1359</v>
       </c>
     </row>
-    <row r="1053" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1053" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1053" t="s">
         <v>1270</v>
       </c>
@@ -30768,7 +30605,7 @@
         <v>1359</v>
       </c>
     </row>
-    <row r="1057" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1057" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1057" t="s">
         <v>1270</v>
       </c>
@@ -30953,7 +30790,7 @@
         <v>1363</v>
       </c>
     </row>
-    <row r="1065" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1065" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1065" t="s">
         <v>1270</v>
       </c>
@@ -31237,7 +31074,7 @@
         <v>1367</v>
       </c>
     </row>
-    <row r="1077" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1077" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1077" t="s">
         <v>1262</v>
       </c>
@@ -31332,7 +31169,7 @@
         <v>1367</v>
       </c>
     </row>
-    <row r="1081" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1081" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1081" t="s">
         <v>1262</v>
       </c>
@@ -31381,7 +31218,7 @@
         <v>1369</v>
       </c>
     </row>
-    <row r="1083" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1083" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1083" t="s">
         <v>1262</v>
       </c>
@@ -31479,7 +31316,7 @@
         <v>1369</v>
       </c>
     </row>
-    <row r="1087" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1087" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1087" t="s">
         <v>1262</v>
       </c>
@@ -31528,7 +31365,7 @@
         <v>1371</v>
       </c>
     </row>
-    <row r="1089" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1089" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1089" t="s">
         <v>1262</v>
       </c>
@@ -31623,7 +31460,7 @@
         <v>1371</v>
       </c>
     </row>
-    <row r="1093" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1093" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1093" t="s">
         <v>1262</v>
       </c>
@@ -31672,7 +31509,7 @@
         <v>1373</v>
       </c>
     </row>
-    <row r="1095" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1095" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1095" t="s">
         <v>1262</v>
       </c>
@@ -31767,7 +31604,7 @@
         <v>1373</v>
       </c>
     </row>
-    <row r="1099" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1099" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1099" t="s">
         <v>1262</v>
       </c>
@@ -31816,7 +31653,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="1101" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1101" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1101" t="s">
         <v>1262</v>
       </c>
@@ -31914,7 +31751,7 @@
         <v>1639</v>
       </c>
     </row>
-    <row r="1105" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1105" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1105" t="s">
         <v>1262</v>
       </c>
@@ -31963,7 +31800,7 @@
         <v>1376</v>
       </c>
     </row>
-    <row r="1107" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1107" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1107" t="s">
         <v>1262</v>
       </c>
@@ -32058,7 +31895,7 @@
         <v>1376</v>
       </c>
     </row>
-    <row r="1111" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1111" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1111" t="s">
         <v>1262</v>
       </c>
@@ -32107,7 +31944,7 @@
         <v>1378</v>
       </c>
     </row>
-    <row r="1113" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1113" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1113" t="s">
         <v>1262</v>
       </c>
@@ -32205,7 +32042,7 @@
         <v>1378</v>
       </c>
     </row>
-    <row r="1117" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1117" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1117" t="s">
         <v>1262</v>
       </c>
@@ -32257,7 +32094,7 @@
         <v>1639</v>
       </c>
     </row>
-    <row r="1119" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1119" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1119" t="s">
         <v>1262</v>
       </c>
@@ -32352,7 +32189,7 @@
         <v>1380</v>
       </c>
     </row>
-    <row r="1123" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1123" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1123" t="s">
         <v>1262</v>
       </c>
@@ -32401,7 +32238,7 @@
         <v>1382</v>
       </c>
     </row>
-    <row r="1125" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1125" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1125" t="s">
         <v>1262</v>
       </c>
@@ -32499,7 +32336,7 @@
         <v>1639</v>
       </c>
     </row>
-    <row r="1129" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1129" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1129" t="s">
         <v>1262</v>
       </c>
@@ -32548,7 +32385,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="1131" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1131" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1131" t="s">
         <v>1262</v>
       </c>
@@ -32649,7 +32486,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="1135" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1135" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1135" t="s">
         <v>1262</v>
       </c>
@@ -32698,7 +32535,7 @@
         <v>1385</v>
       </c>
     </row>
-    <row r="1137" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1137" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1137" t="s">
         <v>1262</v>
       </c>
@@ -32799,7 +32636,7 @@
         <v>1385</v>
       </c>
     </row>
-    <row r="1141" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1141" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1141" t="s">
         <v>1262</v>
       </c>
@@ -32848,7 +32685,7 @@
         <v>1387</v>
       </c>
     </row>
-    <row r="1143" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1143" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1143" t="s">
         <v>1262</v>
       </c>
@@ -32943,7 +32780,7 @@
         <v>1387</v>
       </c>
     </row>
-    <row r="1147" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1147" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1147" t="s">
         <v>1262</v>
       </c>
@@ -32992,7 +32829,7 @@
         <v>1389</v>
       </c>
     </row>
-    <row r="1149" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1149" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1149" t="s">
         <v>1262</v>
       </c>
@@ -34338,7 +34175,7 @@
         <v>1639</v>
       </c>
     </row>
-    <row r="1207" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1207" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1207" t="s">
         <v>1262</v>
       </c>
@@ -35727,7 +35564,7 @@
         <v>1424</v>
       </c>
     </row>
-    <row r="1267" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1267" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1267" t="s">
         <v>1262</v>
       </c>
@@ -35914,7 +35751,7 @@
         <v>1428</v>
       </c>
     </row>
-    <row r="1275" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1275" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1275" t="s">
         <v>1262</v>
       </c>
@@ -36331,7 +36168,7 @@
         <v>1434</v>
       </c>
     </row>
-    <row r="1293" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1293" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1293" t="s">
         <v>1262</v>
       </c>
@@ -38532,9 +38369,6 @@
       </c>
       <c r="G1386" t="s">
         <v>1571</v>
-      </c>
-      <c r="H1386" t="s">
-        <v>1639</v>
       </c>
     </row>
     <row r="1387" spans="1:8" hidden="1" x14ac:dyDescent="0.2">

</xml_diff>